<commit_message>
adding pre-relocations in push-path
</commit_message>
<xml_diff>
--- a/log/data_2o1r_2.xlsx
+++ b/log/data_2o1r_2.xlsx
@@ -501,22 +501,22 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.002902</t>
+          <t>0.003208</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.001321</t>
+          <t>0.001585</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.00024</t>
+          <t>0.000135</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.006244</t>
+          <t>0.00728</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -553,22 +553,22 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.002426</t>
+          <t>0.003666</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.001306</t>
+          <t>0.000612</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.000246</t>
+          <t>0.000129</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.005731</t>
+          <t>0.006954</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -605,22 +605,22 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.002644</t>
+          <t>0.00352</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.00454</t>
+          <t>0.00065</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.000242</t>
+          <t>0.000131</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.009191</t>
+          <t>0.006871</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -657,22 +657,22 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.002389</t>
+          <t>0.003179</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.002888</t>
+          <t>0.001415</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.000222</t>
+          <t>0.000128</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.007195</t>
+          <t>0.007103</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -709,22 +709,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.002362</t>
+          <t>0.002973</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.00273</t>
+          <t>0.001332</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.00023</t>
+          <t>0.000122</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.007019</t>
+          <t>0.006871</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -761,22 +761,22 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.002654</t>
+          <t>0.003798</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.00136</t>
+          <t>0.00055</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.000242</t>
+          <t>0.000132</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.006059</t>
+          <t>0.007022</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -813,22 +813,22 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.001336</t>
+          <t>0.003474</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.000862</t>
+          <t>0.002467</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.000124</t>
+          <t>0.000126</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.00319</t>
+          <t>0.008515</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -865,22 +865,22 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.002635</t>
+          <t>0.00361</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.00134</t>
+          <t>0.001565</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.000243</t>
+          <t>0.000137</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.005932</t>
+          <t>0.007942</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -917,22 +917,22 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0.002809</t>
+          <t>0.003525</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0.005539</t>
+          <t>0.00069</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.000296</t>
+          <t>0.000135</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.010408</t>
+          <t>0.006804</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -969,22 +969,22 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0.002664</t>
+          <t>0.003018</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0.004857</t>
+          <t>0.003432</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.000235</t>
+          <t>0.000117</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.009513</t>
+          <t>0.008629</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1021,22 +1021,22 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0.001812</t>
+          <t>0.003535</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0.000882</t>
+          <t>0.001558</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0.000166</t>
+          <t>0.000135</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.004188</t>
+          <t>0.007546</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1073,22 +1073,22 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0.002659</t>
+          <t>0.003659</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0.001927</t>
+          <t>0.002745</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>0.000241</t>
+          <t>0.000128</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.006509</t>
+          <t>0.009102</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1125,22 +1125,22 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0.002337</t>
+          <t>0.003062</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0.003426</t>
+          <t>0.000567</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0.000226</t>
+          <t>0.000121</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.007689</t>
+          <t>0.00613</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1177,22 +1177,22 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0.003332</t>
+          <t>0.00349</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0.0058</t>
+          <t>0.002095</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0.000287</t>
+          <t>0.000138</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.011605</t>
+          <t>0.008365</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1229,22 +1229,22 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0.002381</t>
+          <t>0.003392</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0.003387</t>
+          <t>0.002063</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0.000242</t>
+          <t>0.000131</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.007709</t>
+          <t>0.00808</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1281,22 +1281,22 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0.002983</t>
+          <t>0.003718</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0.00175</t>
+          <t>0.001489</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>0.00021</t>
+          <t>0.000144</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0.006983</t>
+          <t>0.007991</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1333,22 +1333,22 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0.00237</t>
+          <t>0.00346</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0.001219</t>
+          <t>0.002131</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>0.000213</t>
+          <t>0.000131</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0.005509</t>
+          <t>0.00824</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1385,22 +1385,22 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0.00228</t>
+          <t>0.003484</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0.003373</t>
+          <t>0.001582</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>0.00022</t>
+          <t>0.000124</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0.00756</t>
+          <t>0.007882</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1437,22 +1437,22 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>0.00236</t>
+          <t>0.003503</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0.001695</t>
+          <t>0.00052</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>0.000185</t>
+          <t>0.000124</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>0.005962</t>
+          <t>0.006559</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1489,22 +1489,22 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0.00255</t>
+          <t>0.003483</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0.001685</t>
+          <t>0.000579</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>0.000293</t>
+          <t>0.000144</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0.006692</t>
+          <t>0.006773</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -1541,22 +1541,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>0.002507</t>
+          <t>0.003567</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0.001222</t>
+          <t>0.000548</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>0.000231</t>
+          <t>0.000123</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0.005736</t>
+          <t>0.006798</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -1593,22 +1593,22 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0.002375</t>
+          <t>0.003666</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0.001365</t>
+          <t>0.000586</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>0.000232</t>
+          <t>0.000132</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0.00565</t>
+          <t>0.006906</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -1645,22 +1645,22 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0.002643</t>
+          <t>0.003359</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0.002194</t>
+          <t>0.000498</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>0.000226</t>
+          <t>0.000124</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0.006746</t>
+          <t>0.0065</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -1697,22 +1697,22 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>0.003352</t>
+          <t>0.003553</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>0.003764</t>
+          <t>0.000582</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0.000259</t>
+          <t>0.000116</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0.00918</t>
+          <t>0.007125</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -1749,22 +1749,22 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>0.002648</t>
+          <t>0.003423</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>0.005479</t>
+          <t>0.000553</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>0.000236</t>
+          <t>0.000135</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>0.010145</t>
+          <t>0.006569</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -1801,22 +1801,22 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>0.002665</t>
+          <t>0.003563</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>0.004615</t>
+          <t>0.001775</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>0.000224</t>
+          <t>0.000137</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0.009283</t>
+          <t>0.008067</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -1853,22 +1853,22 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>0.002553</t>
+          <t>0.003188</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>0.006485</t>
+          <t>0.000936</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>0.000284</t>
+          <t>0.00012</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>0.011105</t>
+          <t>0.006734</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -1905,22 +1905,22 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>0.0027</t>
+          <t>0.003396</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0.001387</t>
+          <t>0.00247</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>0.000262</t>
+          <t>0.000132</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0.006062</t>
+          <t>0.008856</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -1957,22 +1957,22 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>0.00262</t>
+          <t>0.003596</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>0.002249</t>
+          <t>0.000592</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>0.000256</t>
+          <t>0.000138</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>0.006832</t>
+          <t>0.006997</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2009,22 +2009,22 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>0.00241</t>
+          <t>0.003715</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>0.002794</t>
+          <t>0.000533</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>0.000229</t>
+          <t>0.000122</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0.007151</t>
+          <t>0.006948</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2061,22 +2061,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>0.002678</t>
+          <t>0.003359</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>0.001377</t>
+          <t>0.000633</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>0.000244</t>
+          <t>0.000151</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>0.006017</t>
+          <t>0.006693</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2113,22 +2113,22 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>0.002562</t>
+          <t>0.003193</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>0.004629</t>
+          <t>0.000592</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>0.000252</t>
+          <t>0.000122</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0.009158</t>
+          <t>0.006461</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2165,22 +2165,22 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>0.002771</t>
+          <t>0.00358</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>0.001499</t>
+          <t>0.000641</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>0.000214</t>
+          <t>0.000133</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>0.006386</t>
+          <t>0.006934</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2217,22 +2217,22 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>0.002325</t>
+          <t>0.003637</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>0.002082</t>
+          <t>0.000553</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>0.000208</t>
+          <t>0.000138</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>0.006291</t>
+          <t>0.006954</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -2269,22 +2269,22 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>0.002641</t>
+          <t>0.003633</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>0.003017</t>
+          <t>0.000602</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>0.000232</t>
+          <t>0.000134</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0.007578</t>
+          <t>0.006968</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -2321,22 +2321,22 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>0.000764</t>
+          <t>0.003587</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>0.000356</t>
+          <t>0.00155</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>6.7e-05</t>
+          <t>0.000117</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>0.001774</t>
+          <t>0.007844</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2373,22 +2373,22 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>0.002525</t>
+          <t>0.003369</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>0.005857</t>
+          <t>0.000659</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>0.000255</t>
+          <t>0.000136</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>0.010359</t>
+          <t>0.006575</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -2425,22 +2425,22 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>0.002356</t>
+          <t>0.003585</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>0.00118</t>
+          <t>0.000519</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>0.000229</t>
+          <t>0.000128</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>0.005521</t>
+          <t>0.006907</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -2477,22 +2477,22 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>0.002635</t>
+          <t>0.00328</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>0.001459</t>
+          <t>0.000642</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>0.000229</t>
+          <t>0.000134</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>0.006042</t>
+          <t>0.006661</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -2529,22 +2529,22 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>0.002388</t>
+          <t>0.003421</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>0.002698</t>
+          <t>0.000491</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>0.000221</t>
+          <t>0.000123</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>0.006998</t>
+          <t>0.006521</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -2581,22 +2581,22 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>0.002428</t>
+          <t>0.003482</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>0.00244</t>
+          <t>0.003819</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>0.000222</t>
+          <t>0.00013</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>0.006784</t>
+          <t>0.01002</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -2633,22 +2633,22 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>0.002696</t>
+          <t>0.003564</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>0.004691</t>
+          <t>0.000605</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>0.000253</t>
+          <t>0.000139</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>0.009518</t>
+          <t>0.006983</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -2685,22 +2685,22 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>0.002583</t>
+          <t>0.003466</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>0.001243</t>
+          <t>0.000554</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>0.000239</t>
+          <t>0.000131</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>0.006072</t>
+          <t>0.006769</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -2737,22 +2737,22 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>0.002599</t>
+          <t>0.003471</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>0.001406</t>
+          <t>0.002263</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>0.000224</t>
+          <t>0.000147</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>0.005949</t>
+          <t>0.008478</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -2789,22 +2789,22 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>0.00255</t>
+          <t>0.003593</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>0.002968</t>
+          <t>0.000505</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>0.000229</t>
+          <t>0.000131</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>0.007472</t>
+          <t>0.006871</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -2841,22 +2841,22 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>0.002538</t>
+          <t>0.00348</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>0.002328</t>
+          <t>0.000546</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>0.00026</t>
+          <t>0.000133</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>0.006829</t>
+          <t>0.006708</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -2893,22 +2893,22 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>0.002389</t>
+          <t>0.003418</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>0.002566</t>
+          <t>0.002233</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>0.00023</t>
+          <t>0.000126</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>0.006867</t>
+          <t>0.008416</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -2945,22 +2945,22 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>0.002784</t>
+          <t>0.00329</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>0.002086</t>
+          <t>0.000598</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>0.000258</t>
+          <t>0.000131</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>0.006878</t>
+          <t>0.006453</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -2997,22 +2997,22 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>0.002549</t>
+          <t>0.003338</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>0.00147</t>
+          <t>0.000632</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>0.000226</t>
+          <t>0.000131</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>0.005965</t>
+          <t>0.006556</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -3049,22 +3049,22 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>0.002664</t>
+          <t>0.003292</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>0.001295</t>
+          <t>0.002161</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>0.000227</t>
+          <t>0.00013</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>0.006008</t>
+          <t>0.008136</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -3101,22 +3101,22 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>0.002435</t>
+          <t>0.003209</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>0.005261</t>
+          <t>0.000618</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>0.000222</t>
+          <t>0.000129</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>0.009601</t>
+          <t>0.006326</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -3153,22 +3153,22 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>0.002372</t>
+          <t>0.003536</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>0.004759</t>
+          <t>0.000614</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>0.000236</t>
+          <t>0.000119</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>0.00914</t>
+          <t>0.006767</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -3205,22 +3205,22 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>0.002423</t>
+          <t>0.003416</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>0.002456</t>
+          <t>0.001959</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>0.000238</t>
+          <t>0.000131</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>0.006826</t>
+          <t>0.008008</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -3257,22 +3257,22 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>0.002374</t>
+          <t>0.003662</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>0.003045</t>
+          <t>0.000546</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>0.000242</t>
+          <t>0.000131</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>0.007396</t>
+          <t>0.006895</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -3309,22 +3309,22 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>0.002548</t>
+          <t>0.00369</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>0.001166</t>
+          <t>0.001851</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>0.000236</t>
+          <t>0.000136</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>0.00585</t>
+          <t>0.00826</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
@@ -3361,22 +3361,22 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>0.002376</t>
+          <t>0.00359</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>0.001217</t>
+          <t>0.000564</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>0.000211</t>
+          <t>0.000138</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>0.0055</t>
+          <t>0.006879</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
@@ -3413,22 +3413,22 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>0.002568</t>
+          <t>0.003604</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>0.005921</t>
+          <t>0.000475</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>0.00025</t>
+          <t>0.000127</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>0.010492</t>
+          <t>0.006548</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
@@ -3465,22 +3465,22 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>0.002487</t>
+          <t>0.003467</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>0.002758</t>
+          <t>0.000529</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>0.000224</t>
+          <t>0.000143</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>0.007157</t>
+          <t>0.006733</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
@@ -3517,22 +3517,22 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>0.002436</t>
+          <t>0.003439</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>0.001105</t>
+          <t>0.003466</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>0.000233</t>
+          <t>0.00013</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>0.005489</t>
+          <t>0.009655</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
@@ -3569,22 +3569,22 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>0.002652</t>
+          <t>0.00366</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>0.002664</t>
+          <t>0.000609</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>0.000232</t>
+          <t>0.000129</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>0.007251</t>
+          <t>0.006883</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
@@ -3621,22 +3621,22 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>0.002578</t>
+          <t>0.003447</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>0.006405</t>
+          <t>0.00064</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>0.000245</t>
+          <t>0.000139</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>0.010956</t>
+          <t>0.006832</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
@@ -3673,22 +3673,22 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>0.002564</t>
+          <t>0.003534</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>0.001004</t>
+          <t>0.002592</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>0.000225</t>
+          <t>0.000132</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>0.005493</t>
+          <t>0.008922</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
@@ -3725,22 +3725,22 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>0.002658</t>
+          <t>0.003305</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>0.001242</t>
+          <t>0.000526</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>0.000224</t>
+          <t>0.000116</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>0.005826</t>
+          <t>0.006428</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
@@ -3777,22 +3777,22 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>0.00287</t>
+          <t>0.003764</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>0.003181</t>
+          <t>0.000544</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>0.000273</t>
+          <t>0.000127</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>0.00823</t>
+          <t>0.006918</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
@@ -3829,22 +3829,22 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>0.00238</t>
+          <t>0.003535</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>0.001183</t>
+          <t>0.000497</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>0.000222</t>
+          <t>0.000119</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>0.005505</t>
+          <t>0.006522</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
@@ -3881,22 +3881,22 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>0.002621</t>
+          <t>0.003536</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>0.002725</t>
+          <t>0.000561</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>0.00022</t>
+          <t>0.000151</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>0.007265</t>
+          <t>0.006732</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
@@ -3933,22 +3933,22 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>0.002521</t>
+          <t>0.003613</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>0.00296</t>
+          <t>0.000577</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>0.000231</t>
+          <t>0.000159</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>0.007464</t>
+          <t>0.006899</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
@@ -3985,22 +3985,22 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>0.002379</t>
+          <t>0.003309</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>0.003539</t>
+          <t>0.000573</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>0.000226</t>
+          <t>0.000131</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>0.007922</t>
+          <t>0.006632</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
@@ -4037,22 +4037,22 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>0.002473</t>
+          <t>0.002228</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>0.001221</t>
+          <t>0.000361</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>0.000249</t>
+          <t>0.00011</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>0.005703</t>
+          <t>0.004341</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
@@ -4089,22 +4089,22 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>0.002354</t>
+          <t>0.003551</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>0.000749</t>
+          <t>0.000538</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>0.000184</t>
+          <t>0.000133</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>0.005041</t>
+          <t>0.006817</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
@@ -4141,22 +4141,22 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>0.002561</t>
+          <t>0.006793</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>0.006239</t>
+          <t>0.001341</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>0.000237</t>
+          <t>0.000179</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>0.010751</t>
+          <t>0.01136</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
@@ -4193,22 +4193,22 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>0.002621</t>
+          <t>0.003333</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>0.001608</t>
+          <t>0.000536</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>0.000242</t>
+          <t>0.000137</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>0.006372</t>
+          <t>0.006447</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
@@ -4245,22 +4245,22 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>0.002439</t>
+          <t>0.003581</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>0.001147</t>
+          <t>0.000498</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>0.000228</t>
+          <t>0.000143</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>0.005529</t>
+          <t>0.006814</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
@@ -4297,22 +4297,22 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>0.00263</t>
+          <t>0.003139</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>0.003045</t>
+          <t>0.000536</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>0.000232</t>
+          <t>0.000119</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>0.00761</t>
+          <t>0.006125</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -4349,22 +4349,22 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>0.002571</t>
+          <t>0.003477</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>0.002353</t>
+          <t>0.000678</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>0.000252</t>
+          <t>0.000146</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>0.006895</t>
+          <t>0.006814</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
@@ -4401,22 +4401,22 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>0.00236</t>
+          <t>0.003525</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>0.001302</t>
+          <t>0.002397</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>0.000247</t>
+          <t>0.00013</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>0.005656</t>
+          <t>0.008624</t>
         </is>
       </c>
       <c r="J77" t="inlineStr">
@@ -4453,22 +4453,22 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>0.002939</t>
+          <t>0.003195</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>0.003231</t>
+          <t>0.000546</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>0.000273</t>
+          <t>0.000125</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>0.008489</t>
+          <t>0.006205</t>
         </is>
       </c>
       <c r="J78" t="inlineStr">
@@ -4505,22 +4505,22 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>0.002382</t>
+          <t>0.003411</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>0.003037</t>
+          <t>0.000506</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>0.000211</t>
+          <t>0.000129</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>0.007294</t>
+          <t>0.00652</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
@@ -4557,22 +4557,22 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>0.002667</t>
+          <t>0.003267</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>0.002507</t>
+          <t>0.000581</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>0.000245</t>
+          <t>0.000129</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>0.007303</t>
+          <t>0.006322</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
@@ -4609,22 +4609,22 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>0.002433</t>
+          <t>0.00363</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>0.004872</t>
+          <t>0.000708</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>0.000262</t>
+          <t>0.000153</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>0.009263</t>
+          <t>0.00712</t>
         </is>
       </c>
       <c r="J81" t="inlineStr">
@@ -4661,22 +4661,22 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>0.002201</t>
+          <t>0.003504</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>0.003332</t>
+          <t>0.000534</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>0.000168</t>
+          <t>0.000146</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>0.007165</t>
+          <t>0.006639</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
@@ -4713,22 +4713,22 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>0.00255</t>
+          <t>0.00334</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>0.002374</t>
+          <t>0.001702</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>0.000216</t>
+          <t>0.00013</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>0.006862</t>
+          <t>0.007561</t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
@@ -4765,22 +4765,22 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>0.002653</t>
+          <t>0.003412</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>0.001338</t>
+          <t>0.000641</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>0.000257</t>
+          <t>0.000137</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>0.005998</t>
+          <t>0.006794</t>
         </is>
       </c>
       <c r="J84" t="inlineStr">
@@ -4817,22 +4817,22 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>0.002589</t>
+          <t>0.003476</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>0.002711</t>
+          <t>0.003374</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>0.000216</t>
+          <t>0.000125</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>0.007278</t>
+          <t>0.0095</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
@@ -4869,22 +4869,22 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>0.002573</t>
+          <t>0.003059</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>0.001287</t>
+          <t>0.000508</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>0.000244</t>
+          <t>0.000134</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>0.005779</t>
+          <t>0.005994</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
@@ -4921,22 +4921,22 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>0.002766</t>
+          <t>0.003432</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>0.001562</t>
+          <t>0.000666</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>0.000271</t>
+          <t>0.000131</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>0.006327</t>
+          <t>0.006857</t>
         </is>
       </c>
       <c r="J87" t="inlineStr">
@@ -4973,22 +4973,22 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>0.002515</t>
+          <t>0.00362</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>0.001978</t>
+          <t>0.001971</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>0.00025</t>
+          <t>0.000133</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>0.006529</t>
+          <t>0.008324</t>
         </is>
       </c>
       <c r="J88" t="inlineStr">
@@ -5025,22 +5025,22 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>0.002628</t>
+          <t>0.003693</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>0.003231</t>
+          <t>0.000592</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>0.000224</t>
+          <t>0.000139</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>0.007804</t>
+          <t>0.006962</t>
         </is>
       </c>
       <c r="J89" t="inlineStr">
@@ -5077,22 +5077,22 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>0.002481</t>
+          <t>0.003189</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>0.002601</t>
+          <t>0.000498</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>0.000262</t>
+          <t>0.000114</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>0.007057</t>
+          <t>0.006196</t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
@@ -5129,22 +5129,22 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>0.002626</t>
+          <t>0.003532</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>0.00126</t>
+          <t>0.003516</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>0.000237</t>
+          <t>0.000131</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>0.005794</t>
+          <t>0.009697</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
@@ -5181,22 +5181,22 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>0.002424</t>
+          <t>0.003633</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>0.001184</t>
+          <t>0.000549</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>0.000241</t>
+          <t>0.000121</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>0.00557</t>
+          <t>0.006797</t>
         </is>
       </c>
       <c r="J92" t="inlineStr">
@@ -5233,22 +5233,22 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>0.002782</t>
+          <t>0.003246</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>0.003291</t>
+          <t>0.000576</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>0.000249</t>
+          <t>0.000128</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>0.008184</t>
+          <t>0.006377</t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
@@ -5285,22 +5285,22 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>0.002416</t>
+          <t>0.003469</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>0.006245</t>
+          <t>0.002281</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>0.000217</t>
+          <t>0.000125</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>0.010565</t>
+          <t>0.008502</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
@@ -5337,22 +5337,22 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>0.002775</t>
+          <t>0.003174</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>0.003838</t>
+          <t>0.001978</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>0.00024</t>
+          <t>0.000119</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>0.0086</t>
+          <t>0.007685</t>
         </is>
       </c>
       <c r="J95" t="inlineStr">
@@ -5389,22 +5389,22 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>0.002391</t>
+          <t>0.003433</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>0.002478</t>
+          <t>0.000642</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>0.000252</t>
+          <t>0.000129</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>0.00684</t>
+          <t>0.006647</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
@@ -5441,22 +5441,22 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>0.001749</t>
+          <t>0.00344</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>0.001809</t>
+          <t>0.000651</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>0.000164</t>
+          <t>0.000135</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>0.004858</t>
+          <t>0.00679</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -5493,22 +5493,22 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>0.002715</t>
+          <t>0.003309</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>0.002564</t>
+          <t>0.000576</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>0.000239</t>
+          <t>0.000118</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>0.007247</t>
+          <t>0.00653</t>
         </is>
       </c>
       <c r="J98" t="inlineStr">
@@ -5545,22 +5545,22 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>0.002774</t>
+          <t>0.003421</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>0.003296</t>
+          <t>0.001554</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>0.000245</t>
+          <t>0.000129</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>0.008232</t>
+          <t>0.007697</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -5597,22 +5597,22 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>0.002344</t>
+          <t>0.003459</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>0.001229</t>
+          <t>0.001495</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>0.000214</t>
+          <t>0.00013</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>0.005441</t>
+          <t>0.007459</t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
@@ -5649,22 +5649,22 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>0.002535</t>
+          <t>0.003289</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>0.001115</t>
+          <t>0.001683</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>0.000225</t>
+          <t>0.000123</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>0.005193</t>
+          <t>0.00755</t>
         </is>
       </c>
       <c r="J101" t="inlineStr">

</xml_diff>